<commit_message>
Updated .slugignore & launched react through flask
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -877,268 +877,268 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>36.69451522827148</v>
+        <v>36.3798942565918</v>
       </c>
       <c r="B2" t="n">
-        <v>0.244892805814743</v>
+        <v>0.2311378717422485</v>
       </c>
       <c r="C2" t="n">
-        <v>33.77376174926758</v>
+        <v>33.12029266357422</v>
       </c>
       <c r="D2" t="n">
-        <v>34.82183837890625</v>
+        <v>34.84400939941406</v>
       </c>
       <c r="E2" t="n">
-        <v>36.02543258666992</v>
+        <v>38.1926383972168</v>
       </c>
       <c r="F2" t="n">
-        <v>2.251670837402344</v>
+        <v>5.072345733642578</v>
       </c>
       <c r="G2" t="n">
-        <v>337.1688537597656</v>
+        <v>132.3363342285156</v>
       </c>
       <c r="H2" t="n">
-        <v>379.8487243652344</v>
+        <v>66.71249389648438</v>
       </c>
       <c r="I2" t="n">
-        <v>283.0395202636719</v>
+        <v>320.8468017578125</v>
       </c>
       <c r="J2" t="n">
-        <v>463.7484741210938</v>
+        <v>247.9119415283203</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8784714341163635</v>
+        <v>0.7433949708938599</v>
       </c>
       <c r="L2" t="n">
-        <v>1.045347094535828</v>
+        <v>1.172901153564453</v>
       </c>
       <c r="M2" t="n">
-        <v>0.04518529772758484</v>
+        <v>0.06797083467245102</v>
       </c>
       <c r="N2" t="n">
-        <v>0.5741928815841675</v>
+        <v>0.5204110741615295</v>
       </c>
       <c r="O2" t="n">
-        <v>1.619150280952454</v>
+        <v>1.092594742774963</v>
       </c>
       <c r="P2" t="n">
-        <v>1.573964953422546</v>
+        <v>1.024623870849609</v>
       </c>
       <c r="Q2" t="n">
-        <v>15.65094566345215</v>
+        <v>11.99386215209961</v>
       </c>
       <c r="R2" t="n">
-        <v>8.810757637023926</v>
+        <v>7.117724418640137</v>
       </c>
       <c r="S2" t="n">
-        <v>9.819575309753418</v>
+        <v>12.80570602416992</v>
       </c>
       <c r="T2" t="n">
-        <v>7.983755111694336</v>
+        <v>10.97202491760254</v>
       </c>
       <c r="U2" t="n">
-        <v>0.487864762544632</v>
+        <v>0.5354536771774292</v>
       </c>
       <c r="V2" t="n">
-        <v>1.292384386062622</v>
+        <v>1.571723461151123</v>
       </c>
       <c r="W2" t="n">
-        <v>15.73081111907959</v>
+        <v>10.09767913818359</v>
       </c>
       <c r="X2" t="n">
-        <v>1.286241769790649</v>
+        <v>2.589601516723633</v>
       </c>
       <c r="Y2" t="n">
-        <v>-1.833918929100037</v>
+        <v>15.44327926635742</v>
       </c>
       <c r="Z2" t="n">
-        <v>-10.96872997283936</v>
+        <v>0.9973151683807373</v>
       </c>
       <c r="AA2" t="n">
-        <v>14.76257419586182</v>
+        <v>13.28406715393066</v>
       </c>
       <c r="AB2" t="n">
-        <v>1.170729041099548</v>
+        <v>1.637460231781006</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.3092649281024933</v>
+        <v>-2.899353742599487</v>
       </c>
       <c r="AD2" t="n">
-        <v>-66.43708038330078</v>
+        <v>-7.929656505584717</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.04067179560661316</v>
+        <v>0.04105398058891296</v>
       </c>
       <c r="AF2" t="n">
-        <v>2.065092086791992</v>
+        <v>1.054503083229065</v>
       </c>
       <c r="AG2" t="n">
-        <v>1.123574495315552</v>
+        <v>1.405201315879822</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.8467060327529907</v>
+        <v>0.7153990864753723</v>
       </c>
       <c r="AI2" t="n">
-        <v>6.136790752410889</v>
+        <v>4.853835105895996</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1.046253800392151</v>
+        <v>1.296501636505127</v>
       </c>
       <c r="AK2" t="n">
-        <v>6.570394515991211</v>
+        <v>5.699641227722168</v>
       </c>
       <c r="AL2" t="n">
-        <v>2.716222047805786</v>
+        <v>2.666948080062866</v>
       </c>
       <c r="AM2" t="n">
-        <v>15.82240200042725</v>
+        <v>22.63392448425293</v>
       </c>
       <c r="AN2" t="n">
-        <v>1.166691780090332</v>
+        <v>0.9566462635993958</v>
       </c>
       <c r="AO2" t="n">
-        <v>628.8585815429688</v>
+        <v>717.261474609375</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.5636367201805115</v>
+        <v>0.5391760468482971</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1131.299438476562</v>
+        <v>1058.71533203125</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.2932689487934113</v>
+        <v>0.3168524503707886</v>
       </c>
       <c r="AS2" t="n">
-        <v>-88.87980651855469</v>
+        <v>-102.5290069580078</v>
       </c>
       <c r="AT2" t="n">
-        <v>-1.094854354858398</v>
+        <v>-0.9027989506721497</v>
       </c>
       <c r="AU2" t="n">
-        <v>1698.47998046875</v>
+        <v>1884.626220703125</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.2118328511714935</v>
+        <v>0.2096151262521744</v>
       </c>
       <c r="AW2" t="n">
-        <v>892.5250854492188</v>
+        <v>809.751220703125</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.5543014407157898</v>
+        <v>0.4383590519428253</v>
       </c>
       <c r="AY2" t="n">
-        <v>-87.89232635498047</v>
+        <v>-102.8067932128906</v>
       </c>
       <c r="AZ2" t="n">
-        <v>-1.031024575233459</v>
+        <v>-0.8393402695655823</v>
       </c>
       <c r="BA2" t="n">
-        <v>2781.49755859375</v>
+        <v>2997.9375</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.1213107034564018</v>
+        <v>0.1051927357912064</v>
       </c>
       <c r="BC2" t="n">
-        <v>901.4579467773438</v>
+        <v>844.0130004882812</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.6338631510734558</v>
+        <v>0.5375494360923767</v>
       </c>
       <c r="BE2" t="n">
-        <v>-89.08489227294922</v>
+        <v>-104.4080657958984</v>
       </c>
       <c r="BF2" t="n">
-        <v>-1.004695773124695</v>
+        <v>-0.8150216341018677</v>
       </c>
       <c r="BG2" t="n">
-        <v>-7.356418132781982</v>
+        <v>-12.93214416503906</v>
       </c>
       <c r="BH2" t="n">
-        <v>-2.028481483459473</v>
+        <v>-1.410694599151611</v>
       </c>
       <c r="BI2" t="n">
-        <v>16.8010139465332</v>
+        <v>21.38112831115723</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.8918241858482361</v>
+        <v>0.7761311531066895</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.1013462617993355</v>
+        <v>0.08713994175195694</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.3150257468223572</v>
+        <v>0.3648333251476288</v>
       </c>
       <c r="BM2" t="n">
-        <v>-0.01222835574299097</v>
+        <v>-0.02833130210638046</v>
       </c>
       <c r="BN2" t="n">
-        <v>-1.447609782218933</v>
+        <v>-0.6479204893112183</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.7820190787315369</v>
+        <v>0.9177460670471191</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.8495128154754639</v>
+        <v>1.076560854911804</v>
       </c>
       <c r="BQ2" t="n">
-        <v>20.80441474914551</v>
+        <v>20.10033226013184</v>
       </c>
       <c r="BR2" t="n">
-        <v>1.017510652542114</v>
+        <v>1.327543377876282</v>
       </c>
       <c r="BS2" t="n">
-        <v>-4.474945068359375</v>
+        <v>13.85799407958984</v>
       </c>
       <c r="BT2" t="n">
-        <v>-5.075962543487549</v>
+        <v>1.125352144241333</v>
       </c>
       <c r="BU2" t="n">
-        <v>17.36009216308594</v>
+        <v>20.47581100463867</v>
       </c>
       <c r="BV2" t="n">
-        <v>1.092755794525146</v>
+        <v>1.108245730400085</v>
       </c>
       <c r="BW2" t="n">
-        <v>-10.57615375518799</v>
+        <v>-15.63738536834717</v>
       </c>
       <c r="BX2" t="n">
-        <v>-1.73272430896759</v>
+        <v>-1.402887344360352</v>
       </c>
       <c r="BY2" t="n">
-        <v>-3.777114391326904</v>
+        <v>-2.609011173248291</v>
       </c>
       <c r="BZ2" t="n">
-        <v>11.31576824188232</v>
+        <v>9.712672233581543</v>
       </c>
       <c r="CA2" t="n">
-        <v>0.03447069227695465</v>
+        <v>0.06369610875844955</v>
       </c>
       <c r="CB2" t="n">
-        <v>0.003040367038920522</v>
+        <v>-0.002465426689013839</v>
       </c>
       <c r="CC2" t="n">
-        <v>0.05175158008933067</v>
+        <v>0.09334204345941544</v>
       </c>
       <c r="CD2" t="n">
-        <v>2.284012079238892</v>
+        <v>2.728731870651245</v>
       </c>
       <c r="CE2" t="n">
-        <v>1.596806406974792</v>
+        <v>2.427184581756592</v>
       </c>
       <c r="CF2" t="n">
-        <v>0.3643749952316284</v>
+        <v>0.2139999866485596</v>
       </c>
       <c r="CG2" t="n">
-        <v>0.2234381437301636</v>
+        <v>0.2148425579071045</v>
       </c>
       <c r="CH2" t="n">
-        <v>0.212777778506279</v>
+        <v>0.18857142329216</v>
       </c>
       <c r="CI2" t="n">
-        <v>0.3096019923686981</v>
+        <v>0.2943238317966461</v>
       </c>
       <c r="CJ2" t="n">
-        <v>-25.84821891784668</v>
+        <v>-21.38953590393066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>